<commit_message>
Upload 100 futures of the 10 of november
</commit_message>
<xml_diff>
--- a/t1_confection/A1_Inputs/A-I_Classifier_Modes_Demand.xlsx
+++ b/t1_confection/A1_Inputs/A-I_Classifier_Modes_Demand.xlsx
@@ -5069,8 +5069,8 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CCDA0DC61E44874FB77B81A0A8C300E4" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="27b2dddd8e7dbb40e638da4098fa8bb9">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9c2c21c4-f980-47d5-be5b-1bb924ee96a2" xmlns:ns3="1b6bb729-2ef5-410d-b4d4-7ced22c361d1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2d3d23b2622c6bf8a24212abcb0f9b2c" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CCDA0DC61E44874FB77B81A0A8C300E4" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="694dc5982778b78571808a8a0bab1175">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9c2c21c4-f980-47d5-be5b-1bb924ee96a2" xmlns:ns3="1b6bb729-2ef5-410d-b4d4-7ced22c361d1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ac46d101c58d29857918b5bc3d6299d1" ns2:_="" ns3:_="">
     <xsd:import namespace="9c2c21c4-f980-47d5-be5b-1bb924ee96a2"/>
     <xsd:import namespace="1b6bb729-2ef5-410d-b4d4-7ced22c361d1"/>
     <xsd:element name="properties">
@@ -5325,5 +5325,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81BBBA6B-B923-4AAA-A954-EDFB957AC3D6}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ABA5DDDF-959C-4B07-AB6F-E6FEC3573736}"/>
 </file>
</xml_diff>